<commit_message>
speeding up code and adding optimization codes 2_1_2018
</commit_message>
<xml_diff>
--- a/Simple Brayton Cycle/minimizing reactor and recuperator/Parameters.xlsx
+++ b/Simple Brayton Cycle/minimizing reactor and recuperator/Parameters.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sondelskir\OneDrive - UW-Madison\nuclear project\Matlab Codes\Simple Brayton Cycle\minimizing reactor and recuperator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sondelski\OneDrive - UW-Madison\nuclear project\Matlab Codes\Simple Brayton Cycle\minimizing reactor and recuperator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="89303D96BA92B2D3DC2D8B9E22955719A9077695" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{F6BAC8D7-B71F-4AFB-B42F-4522D23231CE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{F103240A-B613-4F51-A9AF-671D931B28C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,19 +404,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B65E0-DA60-4331-B38C-644B129CC320}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10.679093849608501</v>
       </c>
@@ -475,7 +475,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11.679093849608501</v>
       </c>
@@ -504,7 +504,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12.679093849608501</v>
       </c>
@@ -533,7 +533,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13.679093849608501</v>
       </c>
@@ -562,7 +562,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14.679093849608501</v>
       </c>
@@ -591,7 +591,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15.679093849608501</v>
       </c>
@@ -620,7 +620,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16.679093849608499</v>
       </c>
@@ -649,7 +649,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17.679093849608499</v>
       </c>
@@ -678,7 +678,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>18.679093849608499</v>
       </c>
@@ -707,7 +707,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19.679093849608499</v>
       </c>
@@ -736,7 +736,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20.679093849608499</v>
       </c>
@@ -765,7 +765,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21.679093849608499</v>
       </c>
@@ -794,7 +794,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22.679093849608499</v>
       </c>
@@ -823,7 +823,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23.679093849608499</v>
       </c>
@@ -852,7 +852,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24.679093849608499</v>
       </c>
@@ -881,7 +881,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25.679093849608499</v>
       </c>
@@ -910,7 +910,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>26.679093849608499</v>
       </c>
@@ -939,7 +939,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>27.679093849608499</v>
       </c>
@@ -968,7 +968,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>28.679093849608499</v>
       </c>
@@ -997,7 +997,7 @@
         <v>17422.927199999998</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>29.679093849608499</v>
       </c>

</xml_diff>